<commit_message>
new Jupyter notebook for ML preprocessing and update to KSI data dictionary
</commit_message>
<xml_diff>
--- a/Dataset/Killed or Seriously Injured Data Features Data - 4326 - evaluated.xlsx
+++ b/Dataset/Killed or Seriously Injured Data Features Data - 4326 - evaluated.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpggpc-my.sharepoint.com/personal/bardhonia_harding_innovapost_com/Documents/Documents/Analytics/module 20/Crash-Detectives/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{A6A6E5B4-F546-4748-8037-4E5C6C0CD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26BFEF42-9201-46CE-B275-6E620138DDAC}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:40009_{A6A6E5B4-F546-4748-8037-4E5C6C0CD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0503501-1E9E-41B5-A582-02465A4D0432}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="7830" windowWidth="15345" windowHeight="7725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Killed or Seriously Injured Dat" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="156">
   <si>
     <t>Column</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Accident Number</t>
   </si>
   <si>
-    <t>Duplicate Accident #'s, the additional rows provide details on each person involved in the accident.  Therea re 10858 duplicate accident #'s and 6002 unique values</t>
-  </si>
-  <si>
     <t>YEAR</t>
   </si>
   <si>
@@ -443,6 +440,54 @@
   </si>
   <si>
     <t>Need to split this string to extract Lat/Long example, {"type": "Point", "coordinates": [-79.40215463, 43.72510266]}</t>
+  </si>
+  <si>
+    <t>Data Decisions</t>
+  </si>
+  <si>
+    <t>Remove duplicate row and only keep the row with the Involvement type of Driver &amp; Owner and then if there are duplicates still remove owner row.  So that there is a unique accident record</t>
+  </si>
+  <si>
+    <t>Duplicate Accident #'s, the additional rows provide details on each person involved in the accident.  Therea re 10858 duplicate accident #'s and 6002 unique values.  The max length is 10 digits</t>
+  </si>
+  <si>
+    <t>Only 2746 rows have offset information</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32 rows classified as Other or Pending.  Remove these rows</t>
+  </si>
+  <si>
+    <t>Categories are not useful for our analysis</t>
+  </si>
+  <si>
+    <t>29 null values remove those rows</t>
+  </si>
+  <si>
+    <t>18 null values remove</t>
+  </si>
+  <si>
+    <t>4 nulls</t>
+  </si>
+  <si>
+    <t>23 nulls rows remove</t>
+  </si>
+  <si>
+    <t>Identifies the role each individual had in the accident.  There is a duplicate accident record for each individual.  This column to be used to delete all duplicate records where the involvement type is not equal to driver or owner.  Could be dropped after accident duplicates are removed</t>
+  </si>
+  <si>
+    <t>What to do about unknown?</t>
+  </si>
+  <si>
+    <t>1612 null records where the row equals in the INVtype vehicle owner or property owner</t>
+  </si>
+  <si>
+    <t>only 713 records and it is only a number series</t>
+  </si>
+  <si>
+    <t>4894 null values + 435 unknown</t>
+  </si>
+  <si>
+    <t>4747 other vehicle types, 2813 null values</t>
   </si>
 </sst>
 </file>
@@ -953,7 +998,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -962,20 +1007,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1331,722 +1382,757 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="110.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="62.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="2" t="s">
+      <c r="E18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="2" t="s">
+      <c r="E20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="5"/>
+      <c r="D24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="2" t="s">
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="2" t="s">
+      <c r="E25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="2" t="s">
+      <c r="E27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="5"/>
+      <c r="D46" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="5"/>
+      <c r="D47" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="5"/>
+      <c r="D48" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="5"/>
+      <c r="D49" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="C50" s="5"/>
       <c r="D50" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B55" s="6"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to data dictionary
</commit_message>
<xml_diff>
--- a/Dataset/Killed or Seriously Injured Data Features Data - 4326 - evaluated.xlsx
+++ b/Dataset/Killed or Seriously Injured Data Features Data - 4326 - evaluated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpggpc-my.sharepoint.com/personal/bardhonia_harding_innovapost_com/Documents/Documents/Analytics/module 20/Crash-Detectives/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:40009_{A6A6E5B4-F546-4748-8037-4E5C6C0CD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0503501-1E9E-41B5-A582-02465A4D0432}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:40009_{A6A6E5B4-F546-4748-8037-4E5C6C0CD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3EFF97F-583F-4F6A-AE26-91DFCF5DAE93}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="7830" windowWidth="15345" windowHeight="7725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Killed or Seriously Injured Dat" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="158">
   <si>
     <t>Column</t>
   </si>
@@ -488,13 +488,19 @@
   </si>
   <si>
     <t>4747 other vehicle types, 2813 null values</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28  DRIVACT          8462 non-null   object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29  DRIVCOND         8464 non-null   object</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,8 +635,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,6 +831,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,7 +1016,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1027,6 +1045,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1384,8 +1407,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1417,7 @@
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="62.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="76" style="3" customWidth="1"/>
     <col min="5" max="5" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1481,7 +1505,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1517,7 +1541,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -1615,7 +1639,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1630,7 +1654,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -1642,7 +1666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -1701,7 +1725,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>61</v>
       </c>
@@ -1717,13 +1741,15 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>66</v>
       </c>
@@ -1746,13 +1772,15 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>71</v>
       </c>
@@ -1760,11 +1788,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -1777,7 +1805,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>75</v>
       </c>
@@ -1791,11 +1819,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="13" t="s">
         <v>79</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1804,12 +1832,15 @@
       <c r="D30" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="E30" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -1818,8 +1849,11 @@
       <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="E31" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>84</v>
       </c>
@@ -1833,7 +1867,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>87</v>
       </c>
@@ -1847,7 +1881,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>90</v>
       </c>
@@ -1861,7 +1895,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
@@ -1875,7 +1909,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
@@ -1889,7 +1923,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
@@ -2137,5 +2171,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ML folder and ML notebooks
</commit_message>
<xml_diff>
--- a/Dataset/Killed or Seriously Injured Data Features Data - 4326 - evaluated.xlsx
+++ b/Dataset/Killed or Seriously Injured Data Features Data - 4326 - evaluated.xlsx
@@ -8,19 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpggpc-my.sharepoint.com/personal/bardhonia_harding_innovapost_com/Documents/Documents/Analytics/module 20/Crash-Detectives/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:40009_{A6A6E5B4-F546-4748-8037-4E5C6C0CD58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3EFF97F-583F-4F6A-AE26-91DFCF5DAE93}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{2F3991E7-D447-4150-B211-3500E523A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14355" yWindow="0" windowWidth="14205" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Killed or Seriously Injured Dat" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Killed or Seriously Injured Dat'!$A$1:$E$55</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="158">
   <si>
     <t>Column</t>
   </si>
@@ -1407,9 +1422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,15 +1709,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
         <v>57</v>
       </c>
@@ -1741,15 +1754,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
         <v>66</v>
       </c>
@@ -2170,7 +2181,314 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC339244-475E-4BB4-BB45-2D5B9CC12CFC}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>